<commit_message>
simplified main dataset. Separated additional information into separate datasets. Added metadata
</commit_message>
<xml_diff>
--- a/data/individual tables/Nurnberger_1930_tbl8.xlsx
+++ b/data/individual tables/Nurnberger_1930_tbl8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pacif\Desktop\Database Creation\Paper_Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://coyotesusd-my.sharepoint.com/personal/jeff_wesner_usd_edu/Documents/USD/Github Projects/TroPhish/data/individual tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7664AC-ACB4-49A8-8F4D-2FAAAD5C4283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{8B7664AC-ACB4-49A8-8F4D-2FAAAD5C4283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3933E522-C630-4CAB-BE56-739FA870E951}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="15780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30555" yWindow="2415" windowWidth="21600" windowHeight="12675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -275,16 +275,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -570,7 +566,7 @@
   <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,67 +688,64 @@
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2">
         <v>17</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2">
         <v>82</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8" t="s">
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8">
+      <c r="K2">
         <v>11</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="6">
         <v>9983</v>
       </c>
-      <c r="M2" s="10">
+      <c r="M2" s="6">
         <v>10106</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" t="s">
         <v>44</v>
       </c>
-      <c r="R2" s="8">
+      <c r="R2">
         <v>1930</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="T2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="U2" t="s">
         <v>49</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="V2" t="s">
         <v>47</v>
       </c>
-      <c r="W2" s="8">
+      <c r="W2">
         <v>1</v>
       </c>
       <c r="Y2" s="2">
@@ -796,29 +789,9 @@
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="T3" s="5"/>
       <c r="Y3" s="3"/>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>

</xml_diff>